<commit_message>
nearly did it !
</commit_message>
<xml_diff>
--- a/Matrice de rigidité K.xlsx
+++ b/Matrice de rigidité K.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2e1e23c5f9e1b181/Documents/Project code/ourocode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{40322A1D-EC32-4438-B07D-6CA17FDA971D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6002908F-95E2-4074-896F-824C6EF9A26B}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{40322A1D-EC32-4438-B07D-6CA17FDA971D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A444DFA8-AE5F-46B3-BBD1-FF780C132ACD}"/>
   <bookViews>
-    <workbookView xWindow="57495" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{860C05A0-E28E-470F-8B3E-9AFCE0901A66}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{860C05A0-E28E-470F-8B3E-9AFCE0901A66}"/>
   </bookViews>
   <sheets>
     <sheet name="Matrice de rigidité K" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1286,10 +1299,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A85AB6-F60C-4C2C-88AD-FE514078316F}">
-  <dimension ref="A1:S19"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2412,6 +2425,12 @@
         <v>250000000</v>
       </c>
     </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <f>H8-B2</f>
+        <v>6250000.0000000009</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>